<commit_message>
tra cuu diem ttth
</commit_message>
<xml_diff>
--- a/TemplateNhapDiemThi.xlsx
+++ b/TemplateNhapDiemThi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieu1\Desktop\CaoThangAngular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\CaoThangAngular\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>hoten</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>laptrinhc</t>
+  </si>
+  <si>
+    <t>0306161291</t>
+  </si>
+  <si>
+    <t>0306161292</t>
   </si>
 </sst>
 </file>
@@ -127,7 +133,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,134 +416,140 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="15.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>123456789</v>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="1">
         <v>36483</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>10</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>123456789</v>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>117215</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>